<commit_message>
added Macros Enabled Excel file
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\P\py\sheet-cutting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5F3B0C-6ADD-4C40-983A-B8C0851FDD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEB56C3-1DF4-4045-86C0-85364B587390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10605" yWindow="1425" windowWidth="17505" windowHeight="13425" xr2:uid="{07E56376-5B08-4B09-80DF-1F05B8431D28}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +91,13 @@
       <sz val="11"/>
       <color rgb="FF111111"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
     </font>

</xml_diff>